<commit_message>
Apply scaling factor to metric values and set endianness.
</commit_message>
<xml_diff>
--- a/src/collector/maps/nexus-metrics.xlsx
+++ b/src/collector/maps/nexus-metrics.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7CE6A7-BF75-40FB-B354-05EDC34C68D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D20E4F-7309-42F1-85FA-58F4C5336134}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Voltage_AN</t>
   </si>
@@ -46,9 +52,6 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>INT16</t>
-  </si>
-  <si>
     <t>Metric Name</t>
   </si>
   <si>
@@ -59,6 +62,12 @@
   </si>
   <si>
     <t>Metric Size</t>
+  </si>
+  <si>
+    <t>INT32</t>
+  </si>
+  <si>
+    <t>Scaling Factor</t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,31 +402,34 @@
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="3" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -430,14 +442,18 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="E2">
+        <f>POWER(2,-16)</f>
+        <v>1.52587890625E-5</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -450,10 +466,14 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="E3">
+        <f>POWER(2,-16)</f>
+        <v>1.52587890625E-5</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove support for string data type and add additional metrics for Nexus meters.
</commit_message>
<xml_diff>
--- a/src/collector/maps/nexus-metrics.xlsx
+++ b/src/collector/maps/nexus-metrics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D20E4F-7309-42F1-85FA-58F4C5336134}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A236770F-4E72-4855-829F-1660A3E694D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Voltage_AN</t>
   </si>
@@ -68,6 +68,183 @@
   </si>
   <si>
     <t>Scaling Factor</t>
+  </si>
+  <si>
+    <t>Voltage_CN</t>
+  </si>
+  <si>
+    <t>1s Phase C-N Voltage</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Voltage_CN</t>
+  </si>
+  <si>
+    <t>Current_N</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Current_N</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>W_A</t>
+  </si>
+  <si>
+    <t>W_B</t>
+  </si>
+  <si>
+    <t>W_C</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>pf_A</t>
+  </si>
+  <si>
+    <t>pf_B</t>
+  </si>
+  <si>
+    <t>pf_C</t>
+  </si>
+  <si>
+    <t>pf</t>
+  </si>
+  <si>
+    <t>Angle_V_AN</t>
+  </si>
+  <si>
+    <t>Angle_V_BN</t>
+  </si>
+  <si>
+    <t>Angle_V_CN</t>
+  </si>
+  <si>
+    <t>Angle_I_A</t>
+  </si>
+  <si>
+    <t>Angle_I_B</t>
+  </si>
+  <si>
+    <t>Angle_I_C</t>
+  </si>
+  <si>
+    <t>1s Frequency</t>
+  </si>
+  <si>
+    <t>1s Phase A Power Factor</t>
+  </si>
+  <si>
+    <t>1s Phase B Power Factor</t>
+  </si>
+  <si>
+    <t>1s Phase C Power Factor</t>
+  </si>
+  <si>
+    <t>1s Three Phase Power Factor</t>
+  </si>
+  <si>
+    <t>1s Neutral Current (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Three Phase Apparent Power (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Three Phase Reactive Power (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Three Phase Active Power (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Phase A Active Power (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Phase B Active Power (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Phase C Active Power (Secondary)</t>
+  </si>
+  <si>
+    <t>1s Phase A-N Voltage Angle</t>
+  </si>
+  <si>
+    <t>1s Phase B-N Voltage Angle</t>
+  </si>
+  <si>
+    <t>1s Phase C-N Voltage Angle</t>
+  </si>
+  <si>
+    <t>1s Phase A Current Angle</t>
+  </si>
+  <si>
+    <t>1s Phase B Current Angle</t>
+  </si>
+  <si>
+    <t>1s Phase C Current Angle</t>
+  </si>
+  <si>
+    <t>UINT16</t>
+  </si>
+  <si>
+    <t>INT16</t>
+  </si>
+  <si>
+    <t>/nexus_meter/VA</t>
+  </si>
+  <si>
+    <t>/nexus_meter/VAR</t>
+  </si>
+  <si>
+    <t>/nexus_meter/W_A</t>
+  </si>
+  <si>
+    <t>/nexus_meter/W_B</t>
+  </si>
+  <si>
+    <t>/nexus_meter/W_C</t>
+  </si>
+  <si>
+    <t>/nexus_meter/W</t>
+  </si>
+  <si>
+    <t>/nexus_meter/freq</t>
+  </si>
+  <si>
+    <t>/nexus_meter/pf_A</t>
+  </si>
+  <si>
+    <t>/nexus_meter/pf_B</t>
+  </si>
+  <si>
+    <t>/nexus_meter/pf_C</t>
+  </si>
+  <si>
+    <t>/nexus_meter/pf</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Angle_V_AN</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Angle_V_BN</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Angle_V_CN</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Angle_I_A</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Angle_I_B</t>
+  </si>
+  <si>
+    <t>/nexus_meter/Angle_I_C</t>
   </si>
 </sst>
 </file>
@@ -394,14 +571,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1"/>
     <col min="3" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" customWidth="1"/>
   </cols>
@@ -477,6 +654,452 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>183</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>POWER(2,-16)</f>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>193</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f>POWER(2,-16)</f>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>209</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E12" si="0">POWER(2,-16)</f>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>217</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>219</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>221</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>223</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>225</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>227</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13">
+        <v>229</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1E-3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>230</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1E-3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>231</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1E-3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>232</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1E-3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>2594</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>2595</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0.01</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>2596</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.01</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20">
+        <v>2597</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0.01</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>2598</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0.01</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <v>2599</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.01</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add an application handler that reads parameters from the environment.
</commit_message>
<xml_diff>
--- a/src/collector/maps/nexus-metrics.xlsx
+++ b/src/collector/maps/nexus-metrics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A236770F-4E72-4855-829F-1660A3E694D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41D4E6-FCBD-46AA-8FF7-F5969FC35CEA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Voltage_AN</t>
   </si>
   <si>
-    <t>/nexus_meter/Voltage_AN</t>
-  </si>
-  <si>
-    <t>Topic Name Suffix</t>
-  </si>
-  <si>
     <t>1s Phase A-N Voltage</t>
   </si>
   <si>
@@ -46,9 +40,6 @@
     <t>1s Phase B-N Voltage</t>
   </si>
   <si>
-    <t>/nexus_meter/Voltage_BN</t>
-  </si>
-  <si>
     <t>Data Type</t>
   </si>
   <si>
@@ -76,15 +67,9 @@
     <t>1s Phase C-N Voltage</t>
   </si>
   <si>
-    <t>/nexus_meter/Voltage_CN</t>
-  </si>
-  <si>
     <t>Current_N</t>
   </si>
   <si>
-    <t>/nexus_meter/Current_N</t>
-  </si>
-  <si>
     <t>VA</t>
   </si>
   <si>
@@ -194,57 +179,6 @@
   </si>
   <si>
     <t>INT16</t>
-  </si>
-  <si>
-    <t>/nexus_meter/VA</t>
-  </si>
-  <si>
-    <t>/nexus_meter/VAR</t>
-  </si>
-  <si>
-    <t>/nexus_meter/W_A</t>
-  </si>
-  <si>
-    <t>/nexus_meter/W_B</t>
-  </si>
-  <si>
-    <t>/nexus_meter/W_C</t>
-  </si>
-  <si>
-    <t>/nexus_meter/W</t>
-  </si>
-  <si>
-    <t>/nexus_meter/freq</t>
-  </si>
-  <si>
-    <t>/nexus_meter/pf_A</t>
-  </si>
-  <si>
-    <t>/nexus_meter/pf_B</t>
-  </si>
-  <si>
-    <t>/nexus_meter/pf_C</t>
-  </si>
-  <si>
-    <t>/nexus_meter/pf</t>
-  </si>
-  <si>
-    <t>/nexus_meter/Angle_V_AN</t>
-  </si>
-  <si>
-    <t>/nexus_meter/Angle_V_BN</t>
-  </si>
-  <si>
-    <t>/nexus_meter/Angle_V_CN</t>
-  </si>
-  <si>
-    <t>/nexus_meter/Angle_I_A</t>
-  </si>
-  <si>
-    <t>/nexus_meter/Angle_I_B</t>
-  </si>
-  <si>
-    <t>/nexus_meter/Angle_I_C</t>
   </si>
 </sst>
 </file>
@@ -571,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,38 +514,34 @@
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="68.140625" customWidth="1"/>
     <col min="3" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>179</v>
@@ -624,18 +554,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>181</v>
@@ -648,18 +575,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
       <c r="C4">
         <v>183</v>
@@ -672,18 +596,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>193</v>
@@ -696,18 +617,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>209</v>
@@ -720,18 +638,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <v>217</v>
@@ -744,18 +659,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>219</v>
@@ -768,18 +680,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>221</v>
@@ -792,18 +701,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>223</v>
@@ -816,18 +722,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>225</v>
@@ -840,18 +743,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>227</v>
@@ -864,18 +764,15 @@
         <v>1.52587890625E-5</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>229</v>
@@ -887,18 +784,15 @@
         <v>1E-3</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>230</v>
@@ -910,18 +804,15 @@
         <v>1E-3</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>231</v>
@@ -933,18 +824,15 @@
         <v>1E-3</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>232</v>
@@ -956,18 +844,15 @@
         <v>1E-3</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>2594</v>
@@ -979,18 +864,15 @@
         <v>0.01</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>2595</v>
@@ -1002,18 +884,15 @@
         <v>0.01</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>2596</v>
@@ -1025,18 +904,15 @@
         <v>0.01</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>2597</v>
@@ -1048,18 +924,15 @@
         <v>0.01</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>2598</v>
@@ -1071,18 +944,15 @@
         <v>0.01</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>2599</v>
@@ -1094,10 +964,7 @@
         <v>0.01</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>